<commit_message>
changed priority_config_beknopt.ini for bodem_template.xlsx
</commit_message>
<xml_diff>
--- a/data/bodem_template_full.xlsx
+++ b/data/bodem_template_full.xlsx
@@ -6852,10 +6852,10 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-07-19 16:18:46.805699</t>
-  </si>
-  <si>
-    <t>Version</t>
+    <t>2024-07-23 17:11:37.581291</t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
   <si>
     <t>1.0.0</t>

</xml_diff>